<commit_message>
added area chart for staff and patients
</commit_message>
<xml_diff>
--- a/app/data/bi_diagramm_data.xlsx
+++ b/app/data/bi_diagramm_data.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jelenanaf/Desktop/SoFa/Normenlos HS25/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jelenanaf/Desktop/final-project-jbns/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD48CA0C-34CC-4942-98BF-362B61990BC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F170CFCE-D765-F642-B4A3-B2468A93C22C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{D262E9B3-518D-A74F-8C4E-03E2C72222A6}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{3BB1FB84-8839-FB4A-82DC-2EADBF823784}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{2589EDF7-73F6-0846-A0FF-71E837D6DF4E}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="45">
   <si>
     <t>Year</t>
   </si>
@@ -159,16 +161,35 @@
   </si>
   <si>
     <t>Cleaning</t>
+  </si>
+  <si>
+    <t>Newborn</t>
+  </si>
+  <si>
+    <t>Children/Teen</t>
+  </si>
+  <si>
+    <t>Adult</t>
+  </si>
+  <si>
+    <t>Elderly</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -194,8 +215,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -530,15 +552,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FC29445-05B9-FA47-BC00-927C51A7C909}">
-  <dimension ref="A1:AC14"/>
+  <dimension ref="A1:AG28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="112" workbookViewId="0">
-      <selection activeCell="Z3" sqref="Z3"/>
+    <sheetView tabSelected="1" zoomScale="161" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
+    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="125" workbookViewId="1"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="2"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -552,82 +576,94 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="J1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="K1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="L1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="M1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="N1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="O1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="P1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="Q1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="R1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="S1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="T1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="U1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="V1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="W1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="X1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="Y1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
+      <c r="Z1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" t="s">
+      <c r="AA1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" t="s">
+      <c r="AB1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AC1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AD1" t="s">
         <v>37</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AE1" t="s">
         <v>38</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AF1" t="s">
         <v>39</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AG1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2024</v>
       </c>
@@ -638,19 +674,21 @@
         <v>22630566</v>
       </c>
       <c r="D2">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="E2">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="F2">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="G2">
-        <v>30</v>
+        <f>V2+90</f>
+        <v>105</v>
       </c>
       <c r="H2">
-        <v>30</v>
+        <f>X2 + 7</f>
+        <v>29</v>
       </c>
       <c r="I2">
         <v>30</v>
@@ -665,58 +703,70 @@
         <v>30</v>
       </c>
       <c r="M2">
+        <v>30</v>
+      </c>
+      <c r="N2">
+        <v>30</v>
+      </c>
+      <c r="O2">
+        <v>30</v>
+      </c>
+      <c r="P2">
+        <v>30</v>
+      </c>
+      <c r="Q2">
         <v>20</v>
       </c>
-      <c r="N2">
+      <c r="R2">
         <v>29</v>
       </c>
-      <c r="O2">
+      <c r="S2">
         <v>19</v>
       </c>
-      <c r="P2">
+      <c r="T2">
         <v>27</v>
       </c>
-      <c r="Q2">
+      <c r="U2">
         <v>24</v>
       </c>
-      <c r="R2">
+      <c r="V2">
         <v>15</v>
       </c>
-      <c r="S2">
+      <c r="W2">
+        <v>14</v>
+      </c>
+      <c r="X2">
+        <v>22</v>
+      </c>
+      <c r="Y2">
         <v>8</v>
       </c>
-      <c r="T2">
+      <c r="Z2">
+        <v>38</v>
+      </c>
+      <c r="AA2">
+        <v>91</v>
+      </c>
+      <c r="AB2">
+        <v>11</v>
+      </c>
+      <c r="AC2">
         <v>22</v>
       </c>
-      <c r="U2">
-        <v>8</v>
-      </c>
-      <c r="V2">
-        <v>34</v>
-      </c>
-      <c r="W2">
-        <v>89</v>
-      </c>
-      <c r="X2">
-        <v>11</v>
-      </c>
-      <c r="Y2">
-        <v>22</v>
-      </c>
-      <c r="Z2">
+      <c r="AD2">
         <v>357</v>
       </c>
-      <c r="AA2">
+      <c r="AE2">
         <v>130</v>
       </c>
-      <c r="AB2">
+      <c r="AF2">
         <v>52</v>
       </c>
-      <c r="AC2">
+      <c r="AG2">
         <v>162</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2025</v>
       </c>
@@ -727,19 +777,22 @@
         <v>22436172</v>
       </c>
       <c r="D3">
-        <v>143</v>
+        <v>165</v>
       </c>
       <c r="E3">
-        <v>30</v>
+        <f>W3</f>
+        <v>19</v>
       </c>
       <c r="F3">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="G3">
-        <v>30</v>
+        <f>V3+86</f>
+        <v>100</v>
       </c>
       <c r="H3">
-        <v>30</v>
+        <f>X3+4</f>
+        <v>27</v>
       </c>
       <c r="I3">
         <v>30</v>
@@ -754,58 +807,70 @@
         <v>30</v>
       </c>
       <c r="M3">
+        <v>30</v>
+      </c>
+      <c r="N3">
+        <v>30</v>
+      </c>
+      <c r="O3">
+        <v>30</v>
+      </c>
+      <c r="P3">
+        <v>30</v>
+      </c>
+      <c r="Q3">
         <v>16</v>
       </c>
-      <c r="N3">
+      <c r="R3">
         <v>21</v>
       </c>
-      <c r="O3">
+      <c r="S3">
         <v>15</v>
       </c>
-      <c r="P3">
+      <c r="T3">
         <v>28</v>
       </c>
-      <c r="Q3">
+      <c r="U3">
         <v>29</v>
       </c>
-      <c r="R3">
+      <c r="V3">
         <v>14</v>
       </c>
-      <c r="S3">
-        <v>7</v>
-      </c>
-      <c r="T3">
-        <v>13</v>
-      </c>
-      <c r="U3">
+      <c r="W3">
+        <v>19</v>
+      </c>
+      <c r="X3">
+        <v>23</v>
+      </c>
+      <c r="Y3">
         <v>8</v>
       </c>
-      <c r="V3">
+      <c r="Z3">
         <v>29</v>
       </c>
-      <c r="W3">
-        <v>79</v>
-      </c>
-      <c r="X3">
-        <v>13</v>
-      </c>
-      <c r="Y3">
+      <c r="AA3">
+        <v>94</v>
+      </c>
+      <c r="AB3">
+        <v>20</v>
+      </c>
+      <c r="AC3">
         <v>14</v>
       </c>
-      <c r="Z3">
+      <c r="AD3">
         <v>351</v>
       </c>
-      <c r="AA3">
+      <c r="AE3">
         <v>130</v>
       </c>
-      <c r="AB3">
+      <c r="AF3">
         <v>50</v>
       </c>
-      <c r="AC3">
+      <c r="AG3">
         <v>163</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2025</v>
       </c>
@@ -816,19 +881,23 @@
         <v>23326502</v>
       </c>
       <c r="D4">
-        <v>145</v>
+        <f>SUM(Q4:X4)</f>
+        <v>158</v>
       </c>
       <c r="E4">
-        <v>30</v>
+        <f t="shared" ref="E4:E14" si="0">W4</f>
+        <v>17</v>
       </c>
       <c r="F4">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="G4">
-        <v>30</v>
+        <f>V4+80</f>
+        <v>92</v>
       </c>
       <c r="H4">
-        <v>30</v>
+        <f>X4+10</f>
+        <v>31</v>
       </c>
       <c r="I4">
         <v>30</v>
@@ -843,58 +912,70 @@
         <v>30</v>
       </c>
       <c r="M4">
+        <v>30</v>
+      </c>
+      <c r="N4">
+        <v>30</v>
+      </c>
+      <c r="O4">
+        <v>30</v>
+      </c>
+      <c r="P4">
+        <v>30</v>
+      </c>
+      <c r="Q4">
         <v>16</v>
       </c>
-      <c r="N4">
+      <c r="R4">
         <v>32</v>
       </c>
-      <c r="O4">
+      <c r="S4">
         <v>12</v>
       </c>
-      <c r="P4">
+      <c r="T4">
         <v>27</v>
       </c>
-      <c r="Q4">
+      <c r="U4">
         <v>21</v>
       </c>
-      <c r="R4">
+      <c r="V4">
         <v>12</v>
       </c>
-      <c r="S4">
-        <v>4</v>
-      </c>
-      <c r="T4">
+      <c r="W4">
+        <v>17</v>
+      </c>
+      <c r="X4">
         <v>21</v>
       </c>
-      <c r="U4">
+      <c r="Y4">
         <v>7</v>
       </c>
-      <c r="V4">
+      <c r="Z4">
         <v>32</v>
       </c>
-      <c r="W4">
-        <v>77</v>
-      </c>
-      <c r="X4">
-        <v>14</v>
-      </c>
-      <c r="Y4">
+      <c r="AA4">
+        <v>85</v>
+      </c>
+      <c r="AB4">
+        <v>19</v>
+      </c>
+      <c r="AC4">
         <v>15</v>
       </c>
-      <c r="Z4">
+      <c r="AD4">
         <v>383</v>
       </c>
-      <c r="AA4">
+      <c r="AE4">
         <v>143</v>
       </c>
-      <c r="AB4">
+      <c r="AF4">
         <v>50</v>
       </c>
-      <c r="AC4">
+      <c r="AG4">
         <v>181</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2025</v>
       </c>
@@ -905,19 +986,23 @@
         <v>23926323</v>
       </c>
       <c r="D5">
-        <v>163</v>
+        <f t="shared" ref="D5:D14" si="1">SUM(Q5:X5)</f>
+        <v>166</v>
       </c>
       <c r="E5">
-        <v>30</v>
+        <f t="shared" si="0"/>
+        <v>13</v>
       </c>
       <c r="F5">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="G5">
-        <v>30</v>
+        <f>V5+88</f>
+        <v>101</v>
       </c>
       <c r="H5">
-        <v>30</v>
+        <f>X5+11</f>
+        <v>32</v>
       </c>
       <c r="I5">
         <v>30</v>
@@ -932,58 +1017,70 @@
         <v>30</v>
       </c>
       <c r="M5">
+        <v>30</v>
+      </c>
+      <c r="N5">
+        <v>30</v>
+      </c>
+      <c r="O5">
+        <v>30</v>
+      </c>
+      <c r="P5">
+        <v>30</v>
+      </c>
+      <c r="Q5">
         <v>26</v>
       </c>
-      <c r="N5">
+      <c r="R5">
         <v>29</v>
       </c>
-      <c r="O5">
+      <c r="S5">
         <v>15</v>
       </c>
-      <c r="P5">
+      <c r="T5">
         <v>20</v>
       </c>
-      <c r="Q5">
+      <c r="U5">
         <v>29</v>
       </c>
-      <c r="R5">
+      <c r="V5">
         <v>13</v>
       </c>
-      <c r="S5">
-        <v>10</v>
-      </c>
-      <c r="T5">
+      <c r="W5">
+        <v>13</v>
+      </c>
+      <c r="X5">
         <v>21</v>
       </c>
-      <c r="U5">
+      <c r="Y5">
         <v>7</v>
       </c>
-      <c r="V5">
+      <c r="Z5">
         <v>38</v>
       </c>
-      <c r="W5">
-        <v>90</v>
-      </c>
-      <c r="X5">
+      <c r="AA5">
+        <v>93</v>
+      </c>
+      <c r="AB5">
         <v>15</v>
       </c>
-      <c r="Y5">
+      <c r="AC5">
         <v>13</v>
       </c>
-      <c r="Z5">
+      <c r="AD5">
         <v>382</v>
       </c>
-      <c r="AA5">
+      <c r="AE5">
         <v>138</v>
       </c>
-      <c r="AB5">
+      <c r="AF5">
         <v>52</v>
       </c>
-      <c r="AC5">
+      <c r="AG5">
         <v>174</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2025</v>
       </c>
@@ -994,19 +1091,23 @@
         <v>22813857</v>
       </c>
       <c r="D6">
-        <v>116</v>
+        <f t="shared" si="1"/>
+        <v>130</v>
       </c>
       <c r="E6">
-        <v>30</v>
+        <f t="shared" si="0"/>
+        <v>9</v>
       </c>
       <c r="F6">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="G6">
-        <v>30</v>
+        <f>V6+70</f>
+        <v>81</v>
       </c>
       <c r="H6">
-        <v>30</v>
+        <f t="shared" ref="H3:H14" si="2">X6</f>
+        <v>18</v>
       </c>
       <c r="I6">
         <v>30</v>
@@ -1021,58 +1122,70 @@
         <v>30</v>
       </c>
       <c r="M6">
+        <v>30</v>
+      </c>
+      <c r="N6">
+        <v>30</v>
+      </c>
+      <c r="O6">
+        <v>30</v>
+      </c>
+      <c r="P6">
+        <v>30</v>
+      </c>
+      <c r="Q6">
         <v>24</v>
       </c>
-      <c r="N6">
+      <c r="R6">
         <v>17</v>
       </c>
-      <c r="O6">
-        <v>8</v>
-      </c>
-      <c r="P6">
+      <c r="S6">
+        <v>18</v>
+      </c>
+      <c r="T6">
         <v>12</v>
       </c>
-      <c r="Q6">
+      <c r="U6">
         <v>21</v>
       </c>
-      <c r="R6">
+      <c r="V6">
         <v>11</v>
       </c>
-      <c r="S6">
-        <v>5</v>
-      </c>
-      <c r="T6">
+      <c r="W6">
+        <v>9</v>
+      </c>
+      <c r="X6">
         <v>18</v>
-      </c>
-      <c r="U6">
-        <v>7</v>
-      </c>
-      <c r="V6">
-        <v>19</v>
-      </c>
-      <c r="W6">
-        <v>61</v>
-      </c>
-      <c r="X6">
-        <v>22</v>
       </c>
       <c r="Y6">
         <v>7</v>
       </c>
       <c r="Z6">
+        <v>20</v>
+      </c>
+      <c r="AA6">
+        <v>71</v>
+      </c>
+      <c r="AB6">
+        <v>22</v>
+      </c>
+      <c r="AC6">
+        <v>10</v>
+      </c>
+      <c r="AD6">
         <v>355</v>
       </c>
-      <c r="AA6">
+      <c r="AE6">
         <v>128</v>
       </c>
-      <c r="AB6">
+      <c r="AF6">
         <v>53</v>
       </c>
-      <c r="AC6">
+      <c r="AG6">
         <v>167</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2025</v>
       </c>
@@ -1083,19 +1196,23 @@
         <v>22528910</v>
       </c>
       <c r="D7">
-        <v>144</v>
+        <f t="shared" si="1"/>
+        <v>148</v>
       </c>
       <c r="E7">
-        <v>30</v>
+        <f t="shared" si="0"/>
+        <v>9</v>
       </c>
       <c r="F7">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G7">
-        <v>30</v>
+        <f>V7+88</f>
+        <v>97</v>
       </c>
       <c r="H7">
-        <v>30</v>
+        <f t="shared" si="2"/>
+        <v>18</v>
       </c>
       <c r="I7">
         <v>30</v>
@@ -1110,58 +1227,70 @@
         <v>30</v>
       </c>
       <c r="M7">
+        <v>30</v>
+      </c>
+      <c r="N7">
+        <v>30</v>
+      </c>
+      <c r="O7">
+        <v>30</v>
+      </c>
+      <c r="P7">
+        <v>30</v>
+      </c>
+      <c r="Q7">
         <v>23</v>
       </c>
-      <c r="N7">
+      <c r="R7">
         <v>25</v>
       </c>
-      <c r="O7">
+      <c r="S7">
         <v>17</v>
       </c>
-      <c r="P7">
+      <c r="T7">
         <v>20</v>
       </c>
-      <c r="Q7">
-        <v>33</v>
-      </c>
-      <c r="R7">
+      <c r="U7">
+        <v>27</v>
+      </c>
+      <c r="V7">
         <v>9</v>
       </c>
-      <c r="S7">
+      <c r="W7">
         <v>9</v>
       </c>
-      <c r="T7">
-        <v>8</v>
-      </c>
-      <c r="U7">
+      <c r="X7">
+        <v>18</v>
+      </c>
+      <c r="Y7">
         <v>12</v>
       </c>
-      <c r="V7">
+      <c r="Z7">
         <v>25</v>
       </c>
-      <c r="W7">
-        <v>77</v>
-      </c>
-      <c r="X7">
+      <c r="AA7">
+        <v>81</v>
+      </c>
+      <c r="AB7">
         <v>19</v>
       </c>
-      <c r="Y7">
+      <c r="AC7">
         <v>11</v>
       </c>
-      <c r="Z7">
+      <c r="AD7">
         <v>358</v>
       </c>
-      <c r="AA7">
+      <c r="AE7">
         <v>127</v>
       </c>
-      <c r="AB7">
+      <c r="AF7">
         <v>55</v>
       </c>
-      <c r="AC7">
+      <c r="AG7">
         <v>159</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2025</v>
       </c>
@@ -1172,85 +1301,101 @@
         <v>22850804</v>
       </c>
       <c r="D8">
+        <f t="shared" si="1"/>
+        <v>143</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="F8">
+        <v>25</v>
+      </c>
+      <c r="G8">
+        <f>V8+70</f>
+        <v>86</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="I8">
+        <v>30</v>
+      </c>
+      <c r="J8">
+        <v>30</v>
+      </c>
+      <c r="K8">
+        <v>30</v>
+      </c>
+      <c r="L8">
+        <v>30</v>
+      </c>
+      <c r="M8">
+        <v>30</v>
+      </c>
+      <c r="N8">
+        <v>30</v>
+      </c>
+      <c r="O8">
+        <v>30</v>
+      </c>
+      <c r="P8">
+        <v>30</v>
+      </c>
+      <c r="Q8">
+        <v>24</v>
+      </c>
+      <c r="R8">
+        <v>27</v>
+      </c>
+      <c r="S8">
+        <v>15</v>
+      </c>
+      <c r="T8">
+        <v>19</v>
+      </c>
+      <c r="U8">
+        <v>10</v>
+      </c>
+      <c r="V8">
+        <v>16</v>
+      </c>
+      <c r="W8">
+        <v>12</v>
+      </c>
+      <c r="X8">
+        <v>20</v>
+      </c>
+      <c r="Y8">
+        <v>12</v>
+      </c>
+      <c r="Z8">
+        <v>33</v>
+      </c>
+      <c r="AA8">
+        <v>67</v>
+      </c>
+      <c r="AB8">
+        <v>20</v>
+      </c>
+      <c r="AC8">
+        <v>11</v>
+      </c>
+      <c r="AD8">
+        <v>355</v>
+      </c>
+      <c r="AE8">
         <v>130</v>
       </c>
-      <c r="E8">
-        <v>30</v>
-      </c>
-      <c r="F8">
-        <v>30</v>
-      </c>
-      <c r="G8">
-        <v>30</v>
-      </c>
-      <c r="H8">
-        <v>30</v>
-      </c>
-      <c r="I8">
-        <v>30</v>
-      </c>
-      <c r="J8">
-        <v>30</v>
-      </c>
-      <c r="K8">
-        <v>30</v>
-      </c>
-      <c r="L8">
-        <v>30</v>
-      </c>
-      <c r="M8">
-        <v>24</v>
-      </c>
-      <c r="N8">
-        <v>27</v>
-      </c>
-      <c r="O8">
-        <v>8</v>
-      </c>
-      <c r="P8">
-        <v>19</v>
-      </c>
-      <c r="Q8">
-        <v>10</v>
-      </c>
-      <c r="R8">
-        <v>16</v>
-      </c>
-      <c r="S8">
-        <v>6</v>
-      </c>
-      <c r="T8">
-        <v>20</v>
-      </c>
-      <c r="U8">
-        <v>12</v>
-      </c>
-      <c r="V8">
-        <v>30</v>
-      </c>
-      <c r="W8">
-        <v>62</v>
-      </c>
-      <c r="X8">
-        <v>15</v>
-      </c>
-      <c r="Y8">
-        <v>11</v>
-      </c>
-      <c r="Z8">
-        <v>355</v>
-      </c>
-      <c r="AA8">
-        <v>130</v>
-      </c>
-      <c r="AB8">
+      <c r="AF8">
         <v>55</v>
       </c>
-      <c r="AC8">
+      <c r="AG8">
         <v>163</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2025</v>
       </c>
@@ -1261,19 +1406,23 @@
         <v>22504849</v>
       </c>
       <c r="D9">
-        <v>122</v>
+        <f t="shared" si="1"/>
+        <v>149</v>
       </c>
       <c r="E9">
-        <v>30</v>
+        <f t="shared" si="0"/>
+        <v>16</v>
       </c>
       <c r="F9">
         <v>30</v>
       </c>
       <c r="G9">
-        <v>30</v>
+        <f>V9+67</f>
+        <v>77</v>
       </c>
       <c r="H9">
-        <v>30</v>
+        <f t="shared" si="2"/>
+        <v>26</v>
       </c>
       <c r="I9">
         <v>30</v>
@@ -1288,58 +1437,70 @@
         <v>30</v>
       </c>
       <c r="M9">
+        <v>30</v>
+      </c>
+      <c r="N9">
+        <v>30</v>
+      </c>
+      <c r="O9">
+        <v>30</v>
+      </c>
+      <c r="P9">
+        <v>30</v>
+      </c>
+      <c r="Q9">
         <v>21</v>
       </c>
-      <c r="N9">
+      <c r="R9">
         <v>24</v>
       </c>
-      <c r="O9">
-        <v>8</v>
-      </c>
-      <c r="P9">
+      <c r="S9">
+        <v>15</v>
+      </c>
+      <c r="T9">
         <v>18</v>
       </c>
-      <c r="Q9">
+      <c r="U9">
         <v>19</v>
       </c>
-      <c r="R9">
+      <c r="V9">
         <v>10</v>
       </c>
-      <c r="S9">
-        <v>6</v>
-      </c>
-      <c r="T9">
+      <c r="W9">
         <v>16</v>
       </c>
-      <c r="U9">
+      <c r="X9">
+        <v>26</v>
+      </c>
+      <c r="Y9">
         <v>7</v>
       </c>
-      <c r="V9">
-        <v>21</v>
-      </c>
-      <c r="W9">
-        <v>72</v>
-      </c>
-      <c r="X9">
-        <v>10</v>
-      </c>
-      <c r="Y9">
-        <v>12</v>
-      </c>
       <c r="Z9">
+        <v>29</v>
+      </c>
+      <c r="AA9">
+        <v>82</v>
+      </c>
+      <c r="AB9">
+        <v>15</v>
+      </c>
+      <c r="AC9">
+        <v>16</v>
+      </c>
+      <c r="AD9">
         <v>357</v>
       </c>
-      <c r="AA9">
+      <c r="AE9">
         <v>131</v>
       </c>
-      <c r="AB9">
+      <c r="AF9">
         <v>55</v>
       </c>
-      <c r="AC9">
+      <c r="AG9">
         <v>164</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2025</v>
       </c>
@@ -1350,18 +1511,22 @@
         <v>23016536</v>
       </c>
       <c r="D10">
-        <v>120</v>
+        <f t="shared" si="1"/>
+        <v>149</v>
       </c>
       <c r="E10">
-        <v>30</v>
+        <f t="shared" si="0"/>
+        <v>15</v>
       </c>
       <c r="F10">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G10">
-        <v>30</v>
+        <f>V10+67</f>
+        <v>75</v>
       </c>
       <c r="H10">
+        <f t="shared" si="2"/>
         <v>30</v>
       </c>
       <c r="I10">
@@ -1377,58 +1542,70 @@
         <v>30</v>
       </c>
       <c r="M10">
+        <v>30</v>
+      </c>
+      <c r="N10">
+        <v>30</v>
+      </c>
+      <c r="O10">
+        <v>30</v>
+      </c>
+      <c r="P10">
+        <v>30</v>
+      </c>
+      <c r="Q10">
         <v>19</v>
       </c>
-      <c r="N10">
+      <c r="R10">
         <v>16</v>
       </c>
-      <c r="O10">
+      <c r="S10">
+        <v>18</v>
+      </c>
+      <c r="T10">
+        <v>21</v>
+      </c>
+      <c r="U10">
+        <v>22</v>
+      </c>
+      <c r="V10">
         <v>8</v>
       </c>
-      <c r="P10">
-        <v>21</v>
-      </c>
-      <c r="Q10">
-        <v>22</v>
-      </c>
-      <c r="R10">
-        <v>8</v>
-      </c>
-      <c r="S10">
-        <v>8</v>
-      </c>
-      <c r="T10">
-        <v>18</v>
-      </c>
-      <c r="U10">
+      <c r="W10">
+        <v>15</v>
+      </c>
+      <c r="X10">
+        <v>30</v>
+      </c>
+      <c r="Y10">
         <v>9</v>
       </c>
-      <c r="V10">
+      <c r="Z10">
         <v>27</v>
       </c>
-      <c r="W10">
-        <v>57</v>
-      </c>
-      <c r="X10">
-        <v>14</v>
-      </c>
-      <c r="Y10">
-        <v>13</v>
-      </c>
-      <c r="Z10">
+      <c r="AA10">
+        <v>77</v>
+      </c>
+      <c r="AB10">
+        <v>19</v>
+      </c>
+      <c r="AC10">
+        <v>17</v>
+      </c>
+      <c r="AD10">
         <v>354</v>
       </c>
-      <c r="AA10">
+      <c r="AE10">
         <v>129</v>
       </c>
-      <c r="AB10">
+      <c r="AF10">
         <v>55</v>
       </c>
-      <c r="AC10">
+      <c r="AG10">
         <v>166</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2025</v>
       </c>
@@ -1439,19 +1616,23 @@
         <v>22806374</v>
       </c>
       <c r="D11">
-        <v>149</v>
+        <f t="shared" si="1"/>
+        <v>158</v>
       </c>
       <c r="E11">
-        <v>30</v>
+        <f t="shared" si="0"/>
+        <v>14</v>
       </c>
       <c r="F11">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="G11">
-        <v>30</v>
+        <f>V11+70</f>
+        <v>85</v>
       </c>
       <c r="H11">
-        <v>30</v>
+        <f>X11 +6</f>
+        <v>34</v>
       </c>
       <c r="I11">
         <v>30</v>
@@ -1466,58 +1647,70 @@
         <v>30</v>
       </c>
       <c r="M11">
+        <v>30</v>
+      </c>
+      <c r="N11">
+        <v>30</v>
+      </c>
+      <c r="O11">
+        <v>30</v>
+      </c>
+      <c r="P11">
+        <v>30</v>
+      </c>
+      <c r="Q11">
         <v>16</v>
       </c>
-      <c r="N11">
+      <c r="R11">
         <v>26</v>
       </c>
-      <c r="O11">
+      <c r="S11">
         <v>13</v>
       </c>
-      <c r="P11">
+      <c r="T11">
         <v>21</v>
       </c>
-      <c r="Q11">
-        <v>35</v>
-      </c>
-      <c r="R11">
+      <c r="U11">
+        <v>25</v>
+      </c>
+      <c r="V11">
         <v>15</v>
       </c>
-      <c r="S11">
-        <v>8</v>
-      </c>
-      <c r="T11">
-        <v>15</v>
-      </c>
-      <c r="U11">
-        <v>8</v>
-      </c>
-      <c r="V11">
+      <c r="W11">
+        <v>14</v>
+      </c>
+      <c r="X11">
+        <v>28</v>
+      </c>
+      <c r="Y11">
+        <v>10</v>
+      </c>
+      <c r="Z11">
         <v>25</v>
       </c>
-      <c r="W11">
-        <v>83</v>
-      </c>
-      <c r="X11">
+      <c r="AA11">
+        <v>90</v>
+      </c>
+      <c r="AB11">
         <v>16</v>
       </c>
-      <c r="Y11">
+      <c r="AC11">
         <v>17</v>
       </c>
-      <c r="Z11">
+      <c r="AD11">
         <v>355</v>
       </c>
-      <c r="AA11">
+      <c r="AE11">
         <v>127</v>
       </c>
-      <c r="AB11">
+      <c r="AF11">
         <v>54</v>
       </c>
-      <c r="AC11">
+      <c r="AG11">
         <v>166</v>
       </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2025</v>
       </c>
@@ -1528,19 +1721,23 @@
         <v>22804053</v>
       </c>
       <c r="D12">
-        <v>139</v>
+        <f t="shared" si="1"/>
+        <v>168</v>
       </c>
       <c r="E12">
-        <v>30</v>
+        <f t="shared" si="0"/>
+        <v>19</v>
       </c>
       <c r="F12">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="G12">
-        <v>30</v>
+        <f>V12+76</f>
+        <v>87</v>
       </c>
       <c r="H12">
-        <v>30</v>
+        <f>X12+20</f>
+        <v>42</v>
       </c>
       <c r="I12">
         <v>30</v>
@@ -1555,58 +1752,70 @@
         <v>30</v>
       </c>
       <c r="M12">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="N12">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="O12">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="P12">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="Q12">
         <v>20</v>
       </c>
       <c r="R12">
+        <v>37</v>
+      </c>
+      <c r="S12">
+        <v>17</v>
+      </c>
+      <c r="T12">
+        <v>22</v>
+      </c>
+      <c r="U12">
+        <v>20</v>
+      </c>
+      <c r="V12">
         <v>11</v>
       </c>
-      <c r="S12">
-        <v>6</v>
-      </c>
-      <c r="T12">
-        <v>16</v>
-      </c>
-      <c r="U12">
-        <v>4</v>
-      </c>
-      <c r="V12">
-        <v>32</v>
-      </c>
       <c r="W12">
-        <v>77</v>
+        <v>19</v>
       </c>
       <c r="X12">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="Y12">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="Z12">
+        <v>33</v>
+      </c>
+      <c r="AA12">
+        <v>83</v>
+      </c>
+      <c r="AB12">
+        <v>28</v>
+      </c>
+      <c r="AC12">
+        <v>17</v>
+      </c>
+      <c r="AD12">
         <v>357</v>
       </c>
-      <c r="AA12">
+      <c r="AE12">
         <v>127</v>
       </c>
-      <c r="AB12">
+      <c r="AF12">
         <v>55</v>
       </c>
-      <c r="AC12">
+      <c r="AG12">
         <v>166</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2025</v>
       </c>
@@ -1617,19 +1826,23 @@
         <v>22750575</v>
       </c>
       <c r="D13">
-        <v>140</v>
+        <f t="shared" si="1"/>
+        <v>167</v>
       </c>
       <c r="E13">
-        <v>30</v>
+        <f t="shared" si="0"/>
+        <v>22</v>
       </c>
       <c r="F13">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="G13">
-        <v>30</v>
+        <f>V13+70</f>
+        <v>88</v>
       </c>
       <c r="H13">
-        <v>30</v>
+        <f>X13+15</f>
+        <v>38</v>
       </c>
       <c r="I13">
         <v>30</v>
@@ -1644,58 +1857,70 @@
         <v>30</v>
       </c>
       <c r="M13">
+        <v>30</v>
+      </c>
+      <c r="N13">
+        <v>30</v>
+      </c>
+      <c r="O13">
+        <v>30</v>
+      </c>
+      <c r="P13">
+        <v>30</v>
+      </c>
+      <c r="Q13">
         <v>13</v>
       </c>
-      <c r="N13">
+      <c r="R13">
         <v>24</v>
       </c>
-      <c r="O13">
+      <c r="S13">
         <v>16</v>
       </c>
-      <c r="P13">
+      <c r="T13">
         <v>27</v>
       </c>
-      <c r="Q13">
+      <c r="U13">
         <v>24</v>
       </c>
-      <c r="R13">
+      <c r="V13">
         <v>18</v>
       </c>
-      <c r="S13">
-        <v>5</v>
-      </c>
-      <c r="T13">
-        <v>13</v>
-      </c>
-      <c r="U13">
-        <v>9</v>
-      </c>
-      <c r="V13">
-        <v>28</v>
-      </c>
       <c r="W13">
-        <v>77</v>
+        <v>22</v>
       </c>
       <c r="X13">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="Y13">
         <v>10</v>
       </c>
       <c r="Z13">
+        <v>28</v>
+      </c>
+      <c r="AA13">
+        <v>97</v>
+      </c>
+      <c r="AB13">
+        <v>19</v>
+      </c>
+      <c r="AC13">
+        <v>13</v>
+      </c>
+      <c r="AD13">
         <v>347</v>
       </c>
-      <c r="AA13">
+      <c r="AE13">
         <v>130</v>
       </c>
-      <c r="AB13">
+      <c r="AF13">
         <v>53</v>
       </c>
-      <c r="AC13">
+      <c r="AG13">
         <v>163</v>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2025</v>
       </c>
@@ -1706,19 +1931,23 @@
         <v>23051003</v>
       </c>
       <c r="D14">
-        <v>141</v>
+        <f t="shared" si="1"/>
+        <v>171</v>
       </c>
       <c r="E14">
-        <v>30</v>
+        <f t="shared" si="0"/>
+        <v>25</v>
       </c>
       <c r="F14">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="G14">
-        <v>30</v>
+        <f>V14+70</f>
+        <v>84</v>
       </c>
       <c r="H14">
-        <v>30</v>
+        <f>X14+20</f>
+        <v>41</v>
       </c>
       <c r="I14">
         <v>30</v>
@@ -1733,56 +1962,104 @@
         <v>30</v>
       </c>
       <c r="M14">
+        <v>30</v>
+      </c>
+      <c r="N14">
+        <v>30</v>
+      </c>
+      <c r="O14">
+        <v>30</v>
+      </c>
+      <c r="P14">
+        <v>30</v>
+      </c>
+      <c r="Q14">
         <v>23</v>
       </c>
-      <c r="N14">
+      <c r="R14">
         <v>29</v>
       </c>
-      <c r="O14">
+      <c r="S14">
         <v>15</v>
       </c>
-      <c r="P14">
+      <c r="T14">
         <v>19</v>
       </c>
-      <c r="Q14">
+      <c r="U14">
         <v>25</v>
       </c>
-      <c r="R14">
+      <c r="V14">
         <v>14</v>
       </c>
-      <c r="S14">
-        <v>5</v>
-      </c>
-      <c r="T14">
-        <v>11</v>
-      </c>
-      <c r="U14">
-        <v>7</v>
-      </c>
-      <c r="V14">
-        <v>40</v>
-      </c>
       <c r="W14">
-        <v>67</v>
+        <v>25</v>
       </c>
       <c r="X14">
+        <v>21</v>
+      </c>
+      <c r="Y14">
         <v>14</v>
       </c>
-      <c r="Y14">
+      <c r="Z14">
+        <v>30</v>
+      </c>
+      <c r="AA14">
+        <v>100</v>
+      </c>
+      <c r="AB14">
+        <v>14</v>
+      </c>
+      <c r="AC14">
         <v>13</v>
       </c>
-      <c r="Z14">
+      <c r="AD14">
         <v>352</v>
       </c>
-      <c r="AA14">
+      <c r="AE14">
         <v>130</v>
       </c>
-      <c r="AB14">
+      <c r="AF14">
         <v>49</v>
       </c>
-      <c r="AC14">
+      <c r="AG14">
         <v>163</v>
       </c>
+    </row>
+    <row r="17" spans="24:24" x14ac:dyDescent="0.2">
+      <c r="X17" s="1"/>
+    </row>
+    <row r="18" spans="24:24" x14ac:dyDescent="0.2">
+      <c r="X18" s="1"/>
+    </row>
+    <row r="19" spans="24:24" x14ac:dyDescent="0.2">
+      <c r="X19" s="1"/>
+    </row>
+    <row r="20" spans="24:24" x14ac:dyDescent="0.2">
+      <c r="X20" s="1"/>
+    </row>
+    <row r="21" spans="24:24" x14ac:dyDescent="0.2">
+      <c r="X21" s="1"/>
+    </row>
+    <row r="22" spans="24:24" x14ac:dyDescent="0.2">
+      <c r="X22" s="1"/>
+    </row>
+    <row r="23" spans="24:24" x14ac:dyDescent="0.2">
+      <c r="X23" s="1"/>
+    </row>
+    <row r="24" spans="24:24" x14ac:dyDescent="0.2">
+      <c r="X24" s="1"/>
+    </row>
+    <row r="25" spans="24:24" x14ac:dyDescent="0.2">
+      <c r="X25" s="1"/>
+    </row>
+    <row r="26" spans="24:24" x14ac:dyDescent="0.2">
+      <c r="X26" s="1"/>
+    </row>
+    <row r="27" spans="24:24" x14ac:dyDescent="0.2">
+      <c r="X27" s="1"/>
+    </row>
+    <row r="28" spans="24:24" x14ac:dyDescent="0.2">
+      <c r="X28" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
tidying up a bit our dashboard
</commit_message>
<xml_diff>
--- a/app/data/bi_diagramm_data.xlsx
+++ b/app/data/bi_diagramm_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jelenanaf/Desktop/final-project-jbns/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{733BB5E5-86FA-C943-93BD-DCE98E2172B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8772EA0-92B6-C447-A74B-44E2A0B36D09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{3BB1FB84-8839-FB4A-82DC-2EADBF823784}"/>
   </bookViews>
@@ -98,18 +98,6 @@
     <t>Beds_Ger_Occ</t>
   </si>
   <si>
-    <t>Raw_diet</t>
-  </si>
-  <si>
-    <t>Soft_diet</t>
-  </si>
-  <si>
-    <t>Normal_diet</t>
-  </si>
-  <si>
-    <t>Diabetic_diet</t>
-  </si>
-  <si>
     <t>Vegetarian/Vegan</t>
   </si>
   <si>
@@ -171,6 +159,18 @@
   </si>
   <si>
     <t>Elderly</t>
+  </si>
+  <si>
+    <t>Raw Diet</t>
+  </si>
+  <si>
+    <t>Soft Diet</t>
+  </si>
+  <si>
+    <t>Normal Diet</t>
+  </si>
+  <si>
+    <t>Diabetic Diet</t>
   </si>
 </sst>
 </file>
@@ -552,8 +552,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FC29445-05B9-FA47-BC00-927C51A7C909}">
   <dimension ref="A1:AG28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" topLeftCell="U1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="AC24" sqref="AC24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -572,16 +572,16 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="H1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -632,31 +632,31 @@
         <v>19</v>
       </c>
       <c r="Y1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC1" t="s">
         <v>20</v>
       </c>
-      <c r="Z1" t="s">
-        <v>21</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>22</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>23</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>24</v>
-      </c>
       <c r="AD1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="AE1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="AF1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="AG1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.2">
@@ -664,7 +664,7 @@
         <v>2024</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C2">
         <v>22630566</v>
@@ -766,7 +766,7 @@
         <v>2025</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C3">
         <v>22436172</v>
@@ -868,7 +868,7 @@
         <v>2025</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C4">
         <v>23326502</v>
@@ -970,7 +970,7 @@
         <v>2025</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C5">
         <v>23926323</v>
@@ -1072,7 +1072,7 @@
         <v>2025</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C6">
         <v>22813857</v>
@@ -1174,7 +1174,7 @@
         <v>2025</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C7">
         <v>22528910</v>
@@ -1276,7 +1276,7 @@
         <v>2025</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C8">
         <v>22850804</v>
@@ -1378,7 +1378,7 @@
         <v>2025</v>
       </c>
       <c r="B9" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C9">
         <v>22504849</v>
@@ -1481,7 +1481,7 @@
         <v>2025</v>
       </c>
       <c r="B10" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C10">
         <v>23016536</v>
@@ -1584,7 +1584,7 @@
         <v>2025</v>
       </c>
       <c r="B11" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C11">
         <v>22806374</v>
@@ -1686,7 +1686,7 @@
         <v>2025</v>
       </c>
       <c r="B12" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C12">
         <v>22804053</v>
@@ -1788,7 +1788,7 @@
         <v>2025</v>
       </c>
       <c r="B13" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C13">
         <v>22750575</v>
@@ -1892,7 +1892,7 @@
         <v>2025</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C14">
         <v>23051003</v>

</xml_diff>

<commit_message>
Adjusting the data for the dashboard
</commit_message>
<xml_diff>
--- a/app/data/bi_diagramm_data.xlsx
+++ b/app/data/bi_diagramm_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jelenanaf/Desktop/final-project-jbns/app/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeremystieger/Documents/5. Semester/Data analysis with Python/Data FP - JBNS/final-project-jbns/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{733BB5E5-86FA-C943-93BD-DCE98E2172B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4A00B2A-9D01-F949-B447-708A699D52DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{3BB1FB84-8839-FB4A-82DC-2EADBF823784}"/>
+    <workbookView xWindow="0" yWindow="780" windowWidth="28800" windowHeight="18000" xr2:uid="{3BB1FB84-8839-FB4A-82DC-2EADBF823784}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -213,9 +213,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -552,8 +553,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FC29445-05B9-FA47-BC00-927C51A7C909}">
   <dimension ref="A1:AG28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" zoomScale="109" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -669,21 +670,21 @@
       <c r="C2">
         <v>22630566</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="2">
         <f t="shared" ref="D2:D3" si="0">SUM(Q2:X2)</f>
-        <v>206</v>
+        <v>221</v>
       </c>
       <c r="E2">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="F2">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G2">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="H2">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="I2">
         <v>30</v>
@@ -710,43 +711,43 @@
         <v>30</v>
       </c>
       <c r="Q2">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="R2">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="S2">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="T2">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="U2">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="V2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="W2">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="X2">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="Y2">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="Z2">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="AA2">
-        <v>91</v>
+        <v>106</v>
       </c>
       <c r="AB2">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="AC2">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="AD2">
         <v>357</v>
@@ -771,18 +772,18 @@
       <c r="C3">
         <v>22436172</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="2">
         <f t="shared" si="0"/>
-        <v>198</v>
+        <v>207</v>
       </c>
       <c r="E3">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F3">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="G3">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="H3">
         <v>38</v>
@@ -818,37 +819,37 @@
         <v>26</v>
       </c>
       <c r="S3">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="T3">
+        <v>27</v>
+      </c>
+      <c r="U3">
+        <v>26</v>
+      </c>
+      <c r="V3">
         <v>24</v>
       </c>
-      <c r="U3">
-        <v>25</v>
-      </c>
-      <c r="V3">
+      <c r="W3">
         <v>23</v>
       </c>
-      <c r="W3">
-        <v>22</v>
-      </c>
       <c r="X3">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="Y3">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="Z3">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="AA3">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="AB3">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="AC3">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="AD3">
         <v>351</v>
@@ -873,15 +874,15 @@
       <c r="C4">
         <v>23326502</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="2">
         <f>SUM(Q4:X4)</f>
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="E4">
         <v>30</v>
       </c>
       <c r="F4">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G4">
         <v>103</v>
@@ -914,7 +915,7 @@
         <v>30</v>
       </c>
       <c r="Q4">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="R4">
         <v>27</v>
@@ -929,28 +930,28 @@
         <v>23</v>
       </c>
       <c r="V4">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="W4">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="X4">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Y4">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="Z4">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="AA4">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="AB4">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="AC4">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="AD4">
         <v>383</v>
@@ -975,9 +976,9 @@
       <c r="C5">
         <v>23926323</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="2">
         <f t="shared" ref="D5:D14" si="1">SUM(Q5:X5)</f>
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E5">
         <v>32</v>
@@ -986,7 +987,7 @@
         <v>24</v>
       </c>
       <c r="G5">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="H5">
         <v>35</v>
@@ -1016,19 +1017,19 @@
         <v>30</v>
       </c>
       <c r="Q5">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="R5">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="S5">
         <v>25</v>
       </c>
       <c r="T5">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="U5">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="V5">
         <v>22</v>
@@ -1037,22 +1038,22 @@
         <v>25</v>
       </c>
       <c r="X5">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="Y5">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="Z5">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="AA5">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="AB5">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="AC5">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="AD5">
         <v>382</v>
@@ -1077,7 +1078,7 @@
       <c r="C6">
         <v>22813857</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="2">
         <f t="shared" si="1"/>
         <v>203</v>
       </c>
@@ -1142,19 +1143,19 @@
         <v>27</v>
       </c>
       <c r="Y6">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="Z6">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="AA6">
-        <v>71</v>
+        <v>103</v>
       </c>
       <c r="AB6">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="AC6">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="AD6">
         <v>355</v>
@@ -1179,21 +1180,21 @@
       <c r="C7">
         <v>22528910</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="2">
         <f t="shared" si="1"/>
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="E7">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F7">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G7">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H7">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I7">
         <v>30</v>
@@ -1226,37 +1227,37 @@
         <v>26</v>
       </c>
       <c r="S7">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="T7">
         <v>24</v>
       </c>
       <c r="U7">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="V7">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="W7">
         <v>25</v>
       </c>
       <c r="X7">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Y7">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="Z7">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="AA7">
-        <v>81</v>
+        <v>95</v>
       </c>
       <c r="AB7">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="AC7">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="AD7">
         <v>358</v>
@@ -1281,9 +1282,9 @@
       <c r="C8">
         <v>22850804</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="2">
         <f t="shared" si="1"/>
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E8">
         <v>36</v>
@@ -1292,7 +1293,7 @@
         <v>26</v>
       </c>
       <c r="G8">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H8">
         <v>32</v>
@@ -1334,7 +1335,7 @@
         <v>25</v>
       </c>
       <c r="U8">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="V8">
         <v>24</v>
@@ -1343,22 +1344,22 @@
         <v>23</v>
       </c>
       <c r="X8">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Y8">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="Z8">
         <v>33</v>
       </c>
       <c r="AA8">
-        <v>67</v>
+        <v>106</v>
       </c>
       <c r="AB8">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="AC8">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="AD8">
         <v>355</v>
@@ -1383,22 +1384,21 @@
       <c r="C9">
         <v>22504849</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="2">
         <f t="shared" si="1"/>
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="E9">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F9">
         <v>22</v>
       </c>
       <c r="G9">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="H9">
-        <f t="shared" ref="H3:H14" si="2">X9</f>
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="I9">
         <v>30</v>
@@ -1428,16 +1428,16 @@
         <v>26</v>
       </c>
       <c r="R9">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="S9">
         <v>23</v>
       </c>
       <c r="T9">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="U9">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="V9">
         <v>25</v>
@@ -1446,22 +1446,22 @@
         <v>22</v>
       </c>
       <c r="X9">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="Y9">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="Z9">
         <v>29</v>
       </c>
       <c r="AA9">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="AB9">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="AC9">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="AD9">
         <v>357</v>
@@ -1486,7 +1486,7 @@
       <c r="C10">
         <v>23016536</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="2">
         <f t="shared" si="1"/>
         <v>206</v>
       </c>
@@ -1500,7 +1500,7 @@
         <v>125</v>
       </c>
       <c r="H10">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="H9:H10" si="2">X10</f>
         <v>29</v>
       </c>
       <c r="I10">
@@ -1552,19 +1552,19 @@
         <v>29</v>
       </c>
       <c r="Y10">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="Z10">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AA10">
-        <v>77</v>
+        <v>110</v>
       </c>
       <c r="AB10">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="AC10">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="AD10">
         <v>354</v>
@@ -1591,19 +1591,19 @@
       </c>
       <c r="D11">
         <f t="shared" si="1"/>
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="E11">
         <v>32</v>
       </c>
       <c r="F11">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="G11">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="H11">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="I11">
         <v>30</v>
@@ -1636,7 +1636,7 @@
         <v>26</v>
       </c>
       <c r="S11">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="T11">
         <v>26</v>
@@ -1645,28 +1645,28 @@
         <v>25</v>
       </c>
       <c r="V11">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="W11">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="X11">
         <v>28</v>
       </c>
       <c r="Y11">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="Z11">
         <v>25</v>
       </c>
       <c r="AA11">
-        <v>90</v>
+        <v>120</v>
       </c>
       <c r="AB11">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="AC11">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="AD11">
         <v>355</v>
@@ -1693,16 +1693,16 @@
       </c>
       <c r="D12">
         <f t="shared" si="1"/>
-        <v>189</v>
+        <v>209</v>
       </c>
       <c r="E12">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F12">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="G12">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="H12">
         <v>36</v>
@@ -1732,43 +1732,43 @@
         <v>30</v>
       </c>
       <c r="Q12">
+        <v>25</v>
+      </c>
+      <c r="R12">
+        <v>27</v>
+      </c>
+      <c r="S12">
+        <v>26</v>
+      </c>
+      <c r="T12">
+        <v>27</v>
+      </c>
+      <c r="U12">
         <v>23</v>
       </c>
-      <c r="R12">
-        <v>27</v>
-      </c>
-      <c r="S12">
-        <v>24</v>
-      </c>
-      <c r="T12">
-        <v>22</v>
-      </c>
-      <c r="U12">
-        <v>20</v>
-      </c>
       <c r="V12">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="W12">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="X12">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="Y12">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="Z12">
         <v>33</v>
       </c>
       <c r="AA12">
-        <v>83</v>
+        <v>105</v>
       </c>
       <c r="AB12">
         <v>28</v>
       </c>
       <c r="AC12">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="AD12">
         <v>357</v>
@@ -1795,21 +1795,19 @@
       </c>
       <c r="D13">
         <f t="shared" si="1"/>
-        <v>200</v>
+        <v>222</v>
       </c>
       <c r="E13">
-        <f t="shared" ref="E4:E14" si="3">W13</f>
         <v>26</v>
       </c>
       <c r="F13">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G13">
-        <v>109</v>
+        <v>124</v>
       </c>
       <c r="H13">
-        <f>X13+15</f>
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="I13">
         <v>30</v>
@@ -1836,43 +1834,43 @@
         <v>30</v>
       </c>
       <c r="Q13">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="R13">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="S13">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="T13">
         <v>27</v>
       </c>
       <c r="U13">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="V13">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="W13">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="X13">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="Y13">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="Z13">
         <v>28</v>
       </c>
       <c r="AA13">
-        <v>97</v>
+        <v>118</v>
       </c>
       <c r="AB13">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="AC13">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="AD13">
         <v>347</v>
@@ -1899,19 +1897,19 @@
       </c>
       <c r="D14">
         <f t="shared" si="1"/>
-        <v>195</v>
+        <v>210</v>
       </c>
       <c r="E14">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F14">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="G14">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="H14">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="I14">
         <v>30</v>
@@ -1938,43 +1936,43 @@
         <v>30</v>
       </c>
       <c r="Q14">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="R14">
         <v>29</v>
       </c>
       <c r="S14">
+        <v>25</v>
+      </c>
+      <c r="T14">
+        <v>26</v>
+      </c>
+      <c r="U14">
+        <v>27</v>
+      </c>
+      <c r="V14">
+        <v>26</v>
+      </c>
+      <c r="W14">
+        <v>26</v>
+      </c>
+      <c r="X14">
+        <v>25</v>
+      </c>
+      <c r="Y14">
         <v>22</v>
       </c>
-      <c r="T14">
+      <c r="Z14">
+        <v>32</v>
+      </c>
+      <c r="AA14">
+        <v>107</v>
+      </c>
+      <c r="AB14">
+        <v>27</v>
+      </c>
+      <c r="AC14">
         <v>24</v>
-      </c>
-      <c r="U14">
-        <v>25</v>
-      </c>
-      <c r="V14">
-        <v>25</v>
-      </c>
-      <c r="W14">
-        <v>24</v>
-      </c>
-      <c r="X14">
-        <v>23</v>
-      </c>
-      <c r="Y14">
-        <v>14</v>
-      </c>
-      <c r="Z14">
-        <v>30</v>
-      </c>
-      <c r="AA14">
-        <v>100</v>
-      </c>
-      <c r="AB14">
-        <v>14</v>
-      </c>
-      <c r="AC14">
-        <v>13</v>
       </c>
       <c r="AD14">
         <v>352</v>

</xml_diff>

<commit_message>
Fixed some merge conflicts with the dashboard data
</commit_message>
<xml_diff>
--- a/app/data/bi_diagramm_data.xlsx
+++ b/app/data/bi_diagramm_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeremystieger/Documents/5. Semester/Data analysis with Python/Data FP - JBNS/final-project-jbns/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4A00B2A-9D01-F949-B447-708A699D52DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B403A3A5-77A0-7B43-ACEC-8326D5BC5AD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="780" windowWidth="28800" windowHeight="18000" xr2:uid="{3BB1FB84-8839-FB4A-82DC-2EADBF823784}"/>
   </bookViews>
@@ -98,18 +98,6 @@
     <t>Beds_Ger_Occ</t>
   </si>
   <si>
-    <t>Raw_diet</t>
-  </si>
-  <si>
-    <t>Soft_diet</t>
-  </si>
-  <si>
-    <t>Normal_diet</t>
-  </si>
-  <si>
-    <t>Diabetic_diet</t>
-  </si>
-  <si>
     <t>Vegetarian/Vegan</t>
   </si>
   <si>
@@ -171,6 +159,18 @@
   </si>
   <si>
     <t>Elderly</t>
+  </si>
+  <si>
+    <t>Raw Diet</t>
+  </si>
+  <si>
+    <t>Soft Diet</t>
+  </si>
+  <si>
+    <t>Normal Diet</t>
+  </si>
+  <si>
+    <t>Diabetic Diet</t>
   </si>
 </sst>
 </file>
@@ -213,10 +213,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -553,8 +552,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FC29445-05B9-FA47-BC00-927C51A7C909}">
   <dimension ref="A1:AG28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="109" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="109" workbookViewId="0">
+      <selection activeCell="AB2" sqref="AB2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -573,16 +572,16 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="H1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
@@ -633,31 +632,31 @@
         <v>19</v>
       </c>
       <c r="Y1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC1" t="s">
         <v>20</v>
       </c>
-      <c r="Z1" t="s">
-        <v>21</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>22</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>23</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>24</v>
-      </c>
       <c r="AD1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="AE1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="AF1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="AG1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.2">
@@ -665,12 +664,12 @@
         <v>2024</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C2">
         <v>22630566</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2">
         <f t="shared" ref="D2:D3" si="0">SUM(Q2:X2)</f>
         <v>221</v>
       </c>
@@ -767,12 +766,12 @@
         <v>2025</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C3">
         <v>22436172</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3">
         <f t="shared" si="0"/>
         <v>207</v>
       </c>
@@ -869,12 +868,12 @@
         <v>2025</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C4">
         <v>23326502</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4">
         <f>SUM(Q4:X4)</f>
         <v>204</v>
       </c>
@@ -971,12 +970,12 @@
         <v>2025</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C5">
         <v>23926323</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5">
         <f t="shared" ref="D5:D14" si="1">SUM(Q5:X5)</f>
         <v>203</v>
       </c>
@@ -1073,12 +1072,12 @@
         <v>2025</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C6">
         <v>22813857</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6">
         <f t="shared" si="1"/>
         <v>203</v>
       </c>
@@ -1175,12 +1174,12 @@
         <v>2025</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C7">
         <v>22528910</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7">
         <f t="shared" si="1"/>
         <v>196</v>
       </c>
@@ -1277,12 +1276,12 @@
         <v>2025</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C8">
         <v>22850804</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8">
         <f t="shared" si="1"/>
         <v>204</v>
       </c>
@@ -1379,12 +1378,12 @@
         <v>2025</v>
       </c>
       <c r="B9" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C9">
         <v>22504849</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9">
         <f t="shared" si="1"/>
         <v>194</v>
       </c>
@@ -1481,12 +1480,12 @@
         <v>2025</v>
       </c>
       <c r="B10" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C10">
         <v>23016536</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10">
         <f t="shared" si="1"/>
         <v>206</v>
       </c>
@@ -1500,7 +1499,7 @@
         <v>125</v>
       </c>
       <c r="H10">
-        <f t="shared" ref="H9:H10" si="2">X10</f>
+        <f t="shared" ref="H10" si="2">X10</f>
         <v>29</v>
       </c>
       <c r="I10">
@@ -1584,7 +1583,7 @@
         <v>2025</v>
       </c>
       <c r="B11" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C11">
         <v>22806374</v>
@@ -1686,7 +1685,7 @@
         <v>2025</v>
       </c>
       <c r="B12" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C12">
         <v>22804053</v>
@@ -1788,7 +1787,7 @@
         <v>2025</v>
       </c>
       <c r="B13" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C13">
         <v>22750575</v>
@@ -1890,7 +1889,7 @@
         <v>2025</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C14">
         <v>23051003</v>

</xml_diff>